<commit_message>
feat(tab6): hybrid export engine — auto-tagging + xlsx-template for perfect row cloning
</commit_message>
<xml_diff>
--- a/mock_supplier_template.xlsx
+++ b/mock_supplier_template.xlsx
@@ -1,47 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Order Form" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Purchase Order" state="visible" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+  <si>
+    <t>Huma Medical Production Co. Ltd</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PURCHASE ORDER</t>
+  </si>
+  <si>
+    <t>Your Health, Our Care</t>
+  </si>
+  <si>
+    <t>DATE: 2024-01-19</t>
+  </si>
+  <si>
+    <t>BILL TO</t>
+  </si>
+  <si>
+    <t>SHIP TO</t>
+  </si>
+  <si>
+    <t>HSC JAPAN JOINT STOCK COMPANY</t>
+  </si>
+  <si>
+    <t>HUMA MEDICAL HANOI</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Item Code</t>
+  </si>
+  <si>
+    <t>Item name/Package</t>
+  </si>
+  <si>
+    <t>Pkg</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>SUBTOTAL</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>TAX</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -60,18 +102,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,32 +463,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>品名</v>
-      </c>
-      <c r="B1" t="str">
-        <v>数量</v>
-      </c>
-      <c r="C1" t="str">
-        <v>単価</v>
-      </c>
-      <c r="D1" t="str">
-        <v>納期</v>
-      </c>
-      <c r="E1" t="str">
-        <v>備考</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>